<commit_message>
AddCompanies, AddAuth, Add Vacancies Creation
</commit_message>
<xml_diff>
--- a/ProcessAuto/Companies.xlsx
+++ b/ProcessAuto/Companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ukwim\Documents\GitHub\Projects\ProcessAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A96FAF-177B-46C1-8DD2-A744A8783BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAD7C22-55C0-4732-8B74-3102B78B4E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,12 +372,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="4" max="4" width="21.1015625" customWidth="1"/>
+    <col min="5" max="5" width="12.26171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>